<commit_message>
retrain predict transport model modify divide places code
</commit_message>
<xml_diff>
--- a/TestSv/static/predict_transport.xlsx
+++ b/TestSv/static/predict_transport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCMUS\CNTT\DA_TN\Test\crawl_tour\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCMUS\CNTT\DA_TN\Test\TestSv\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDE0522-EDAB-4192-A9FB-CE0BAAECEBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A8A81E-8DCD-459E-9CDF-8A9F98AB754F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$B$1:$B$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$B$1:$B$38</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="46">
   <si>
     <t>from</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>Thanh Hóa</t>
-  </si>
-  <si>
-    <t>Nghệ An</t>
   </si>
   <si>
     <t>Ninh Bình</t>
@@ -170,7 +167,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +187,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -216,10 +221,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -236,8 +242,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -541,10 +551,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E35" sqref="E28:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,16 +843,16 @@
     </row>
     <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3">
         <v>4</v>
-      </c>
-      <c r="D17" s="4">
-        <v>4.8</v>
       </c>
       <c r="E17" t="s">
         <v>14</v>
@@ -853,13 +863,13 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3">
         <v>3</v>
       </c>
-      <c r="D18" s="3">
-        <v>4</v>
+      <c r="D18" s="4">
+        <v>3.2</v>
       </c>
       <c r="E18" t="s">
         <v>14</v>
@@ -870,16 +880,19 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C19" s="3">
         <v>3</v>
       </c>
       <c r="D19" s="4">
-        <v>3.2</v>
+        <v>2.7</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -887,16 +900,16 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C20" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" s="4">
-        <v>2.7</v>
+        <v>1.9</v>
       </c>
       <c r="E20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>23</v>
@@ -907,16 +920,16 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C21" s="3">
         <v>2</v>
       </c>
       <c r="D21" s="4">
-        <v>1.9</v>
+        <v>2.5</v>
       </c>
       <c r="E21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>24</v>
@@ -927,16 +940,16 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C22" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22" s="4">
-        <v>2.5</v>
+        <v>2.9</v>
       </c>
       <c r="E22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>25</v>
@@ -947,19 +960,19 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C23" s="3">
         <v>3</v>
       </c>
       <c r="D23" s="4">
-        <v>2.9</v>
+        <v>3.8</v>
       </c>
       <c r="E23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -967,16 +980,16 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C24" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D24" s="4">
-        <v>3.8</v>
+        <v>5.5</v>
       </c>
       <c r="E24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>28</v>
@@ -990,13 +1003,13 @@
         <v>13</v>
       </c>
       <c r="C25" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25" s="4">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="E25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>29</v>
@@ -1007,16 +1020,16 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C26" s="3">
         <v>3</v>
       </c>
       <c r="D26" s="4">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="E26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>30</v>
@@ -1027,16 +1040,16 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C27" s="3">
         <v>3</v>
       </c>
       <c r="D27" s="4">
-        <v>3.5</v>
+        <v>2.9</v>
       </c>
       <c r="E27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>31</v>
@@ -1047,39 +1060,39 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C28" s="3">
         <v>3</v>
       </c>
       <c r="D28" s="4">
-        <v>2.9</v>
+        <v>4.2</v>
       </c>
       <c r="E28" t="s">
-        <v>22</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C29" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29" s="4">
-        <v>4.2</v>
+        <v>1.9</v>
       </c>
       <c r="E29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1087,16 +1100,16 @@
         <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D30" s="4">
-        <v>1.9</v>
+        <v>2.6</v>
       </c>
       <c r="E30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>36</v>
@@ -1107,16 +1120,16 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D31" s="4">
-        <v>2.6</v>
+        <v>1.5</v>
       </c>
       <c r="E31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>37</v>
@@ -1127,16 +1140,16 @@
         <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" s="4">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="E32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>38</v>
@@ -1147,56 +1160,56 @@
         <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C33" s="3">
         <v>3</v>
       </c>
       <c r="D33" s="4">
-        <v>2.5</v>
+        <v>4.3</v>
       </c>
       <c r="E33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C34" s="3">
         <v>3</v>
       </c>
       <c r="D34" s="4">
-        <v>4.3</v>
+        <v>3.3</v>
       </c>
       <c r="E34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C35" s="3">
         <v>3</v>
       </c>
       <c r="D35" s="4">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="E35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>43</v>
@@ -1204,19 +1217,19 @@
     </row>
     <row r="36" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C36" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" s="4">
-        <v>3.4</v>
+        <v>1.3</v>
       </c>
       <c r="E36" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>44</v>
@@ -1227,19 +1240,19 @@
         <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" s="3">
         <v>2</v>
       </c>
       <c r="D37" s="4">
-        <v>1.3</v>
+        <v>0.9</v>
       </c>
       <c r="E37" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1247,13 +1260,13 @@
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D38" s="4">
-        <v>0.9</v>
+        <v>4.7</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
@@ -1262,27 +1275,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="3">
-        <v>4</v>
-      </c>
-      <c r="D39" s="4">
-        <v>4.7</v>
-      </c>
-      <c r="E39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F28" r:id="rId1" xr:uid="{AECEF4D0-9D50-4873-9728-E199E8C0F4CC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add vkg iata code
</commit_message>
<xml_diff>
--- a/TestSv/static/predict_transport.xlsx
+++ b/TestSv/static/predict_transport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCMUS\CNTT\DA_TN\Test\TestSv\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A8A81E-8DCD-459E-9CDF-8A9F98AB754F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A24332E-5D6D-4D26-A716-FAED20F4FD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="48">
   <si>
     <t>from</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>https://www.kynghidongduong.vn/tours/tour-du-lich-sapa-ha-giang-tay-bac-dong-bac-lien-tuyen-dong-tay-bac-4-ngay-4-dem-5-ngay-4-dem-tour-sapa-tour-ha-giang-khoi-hanh-tu-ha-noi-gia-re-dich-vu-chat-luong.html</t>
+  </si>
+  <si>
+    <t>Thừa Thiên Huế</t>
+  </si>
+  <si>
+    <t>https://tour.dulichvietnam.com.vn/chi-tiet-tour/68/du-lich-hue-tu-ha-noi-3-ngay.html</t>
   </si>
 </sst>
 </file>
@@ -225,7 +231,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -243,6 +249,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -551,10 +560,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E35" sqref="E28:E35"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -906,7 +915,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="4">
-        <v>1.9</v>
+        <v>2.4</v>
       </c>
       <c r="E20" t="s">
         <v>21</v>
@@ -1086,12 +1095,12 @@
         <v>2</v>
       </c>
       <c r="D29" s="4">
-        <v>1.9</v>
+        <v>2.5</v>
       </c>
       <c r="E29" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="6" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1111,7 +1120,7 @@
       <c r="E30" t="s">
         <v>21</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1126,12 +1135,12 @@
         <v>2</v>
       </c>
       <c r="D31" s="4">
-        <v>1.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E31" t="s">
         <v>21</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1275,9 +1284,33 @@
         <v>45</v>
       </c>
     </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="1">
+        <v>3</v>
+      </c>
+      <c r="D39" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F28" r:id="rId1" xr:uid="{AECEF4D0-9D50-4873-9728-E199E8C0F4CC}"/>
+    <hyperlink ref="F29" r:id="rId2" xr:uid="{D1B01BA7-23A3-4FAC-B191-0E1FCAED897B}"/>
+    <hyperlink ref="F30" r:id="rId3" xr:uid="{55F16A03-B6DC-48C9-86DF-395A6A96672E}"/>
+    <hyperlink ref="F31" r:id="rId4" xr:uid="{A97C9F14-8438-47DF-B820-FD9B133DB57F}"/>
+    <hyperlink ref="F39" r:id="rId5" xr:uid="{2C0748CE-F5BB-4A82-BE8B-2429BF99E48D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
update train data + model
</commit_message>
<xml_diff>
--- a/TestSv/static/predict_transport.xlsx
+++ b/TestSv/static/predict_transport.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCMUS\CNTT\DA_TN\Test\TestSv\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B4CE2E-55C1-42C1-8D07-C3DD19955479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3048" yWindow="1992" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3048" yWindow="1992" windowWidth="17280" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +17,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$B$1:$B$38</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="66">
   <si>
     <t>from</t>
   </si>
@@ -170,13 +169,64 @@
   </si>
   <si>
     <t>https://www.vietnambooking.com/du-lich/tour-nha-trang-3-ngay-2-dem.html</t>
+  </si>
+  <si>
+    <t>Du lịch Hè - Tour Đà Nẵng - Huế - Thánh Địa La Vang - Động Thiên Đường từ Sài Gòn 2023 (dulichviet.com.vn)</t>
+  </si>
+  <si>
+    <t>Du lịch Hè - Tour Du lịch Hà Nội - Sapa - Fansipan từ Sài Gòn 2023 (dulichviet.com.vn)</t>
+  </si>
+  <si>
+    <t>Du lịch Hà Nội - Quảng Bình - Động Phong Nha - Bãi Đá Nhảy - Hang Tám Cô dịp Hè từ Hà Nội 2023 (dulichviet.com.vn)</t>
+  </si>
+  <si>
+    <t>Du lịch Hè - Tour Du lịch Quy Nhơn - Phú Yên từ Hà Nội 2023 (dulichviet.com.vn)</t>
+  </si>
+  <si>
+    <t>Du lịch Hè - Tour Du lịch Hà Nội - Đà Nẵng - Bà Nà - Hội An (dulichviet.com.vn)</t>
+  </si>
+  <si>
+    <t>Du lịch Hè Tour Du lịch Phú Quốc Khám phá Đảo Ngọc từ Hà Nội 2023 (dulichviet.com.vn)</t>
+  </si>
+  <si>
+    <t>Nghệ An</t>
+  </si>
+  <si>
+    <t>Tour Cửa Lò 3 Ngày 2 Đêm giá tốt - Vivu Tour</t>
+  </si>
+  <si>
+    <t>Tour Đà Nẵng - Bà Nà - Hội An - Ngũ Hành Sơn từ TP.HCM 3N2Đ (vietnambooking.com)</t>
+  </si>
+  <si>
+    <t>Bà Rịa - Vũng Tàu</t>
+  </si>
+  <si>
+    <t>Tour Long Hải teambuilding Gala Dinner 2 ngày 1 đêm siêu hấp dẫn (vietnambooking.com)</t>
+  </si>
+  <si>
+    <t>Gia Lai</t>
+  </si>
+  <si>
+    <t>Liên tuyến Tây Nguyên Đắk Nông - Đắk Lắk - Gia Lai - Kon Tum - Lâm Đồng 5N4Đ (viettourist.com)</t>
+  </si>
+  <si>
+    <t>Tour Phan Thiết vườn nho 3 ngày 2 đêm - TeamBuilding - Gala (dulichvietdu.com)</t>
+  </si>
+  <si>
+    <t>Tour du lịch Mũi Né bằng Tàu Hỏa 3 sao 3N2Đ Vietnambooking</t>
+  </si>
+  <si>
+    <t>Hải Phòng</t>
+  </si>
+  <si>
+    <t>Du lịch Hà Nội - Hòn Dấu Resort 2 Ngày 1 Đêm giá tốt (saoviettravel.com.vn)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +254,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -234,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -255,6 +311,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -559,14 +625,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1327,14 +1393,274 @@
         <v>48</v>
       </c>
     </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="9">
+        <v>5</v>
+      </c>
+      <c r="D41" s="10">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="9">
+        <v>3</v>
+      </c>
+      <c r="D42" s="10">
+        <v>7.4</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="9">
+        <v>3</v>
+      </c>
+      <c r="D43" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="9">
+        <v>4</v>
+      </c>
+      <c r="D44" s="10">
+        <v>6.5</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="9">
+        <v>4</v>
+      </c>
+      <c r="D45" s="10">
+        <v>5.7</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="9">
+        <v>4</v>
+      </c>
+      <c r="D46" s="10">
+        <v>6.7</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="9">
+        <v>3</v>
+      </c>
+      <c r="D47" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="9">
+        <v>3</v>
+      </c>
+      <c r="D48" s="10">
+        <v>6.2</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="9">
+        <v>2</v>
+      </c>
+      <c r="D49" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="9">
+        <v>5</v>
+      </c>
+      <c r="D50" s="10">
+        <v>7.8</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="9">
+        <v>3</v>
+      </c>
+      <c r="D51" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="9">
+        <v>3</v>
+      </c>
+      <c r="D52" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="9">
+        <v>2</v>
+      </c>
+      <c r="D53" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F28" r:id="rId1" xr:uid="{AECEF4D0-9D50-4873-9728-E199E8C0F4CC}"/>
-    <hyperlink ref="F29" r:id="rId2" xr:uid="{D1B01BA7-23A3-4FAC-B191-0E1FCAED897B}"/>
-    <hyperlink ref="F30" r:id="rId3" xr:uid="{55F16A03-B6DC-48C9-86DF-395A6A96672E}"/>
-    <hyperlink ref="F31" r:id="rId4" xr:uid="{A97C9F14-8438-47DF-B820-FD9B133DB57F}"/>
-    <hyperlink ref="F39" r:id="rId5" xr:uid="{2C0748CE-F5BB-4A82-BE8B-2429BF99E48D}"/>
-    <hyperlink ref="F40" r:id="rId6" xr:uid="{77BCC1E1-DD67-4D3C-9616-2E787770C8E7}"/>
+    <hyperlink ref="F28" r:id="rId1"/>
+    <hyperlink ref="F29" r:id="rId2"/>
+    <hyperlink ref="F30" r:id="rId3"/>
+    <hyperlink ref="F31" r:id="rId4"/>
+    <hyperlink ref="F39" r:id="rId5"/>
+    <hyperlink ref="F40" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>